<commit_message>
modify the detailUserActivity for the user info
</commit_message>
<xml_diff>
--- a/doc/TouchCalc.xlsx
+++ b/doc/TouchCalc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="10470"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="18195" windowHeight="10470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +71,26 @@
   </si>
   <si>
     <t>&lt;해답&gt; after the drop function has processed you have to create the table again</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SecretManager와 DetailUserActivity간의 통신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>putExtra 사용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단순하게 이름과 전화번호만 필요하다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -507,12 +527,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>